<commit_message>
Correlation files and excel file
Correlation files regrouped

overall correlation excel file - combined 'homework giving' and 'correcting' tab into single columns
</commit_message>
<xml_diff>
--- a/datasets/nas/Correlation Folder/All Combined Correlation.xlsx
+++ b/datasets/nas/Correlation Folder/All Combined Correlation.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\odrive\Amazon Cloud Drive\Documents\NID\SEM 4\data-artistry-tournament\datasets\nas\Correlation Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aromal\Documents\GitHub\data-artistry-tournament\datasets\nas\Correlation Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="General Corr" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="73">
   <si>
     <t>STUID</t>
   </si>
@@ -243,6 +243,12 @@
   <si>
     <t>Topper Reading</t>
   </si>
+  <si>
+    <t>Give Hw</t>
+  </si>
+  <si>
+    <t>Correct HW</t>
+  </si>
 </sst>
 </file>
 
@@ -345,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -353,123 +359,16 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3186,28 +3085,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD5"/>
+  <dimension ref="A1:AX28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="18" max="18" width="8.44140625" customWidth="1"/>
-    <col min="26" max="26" width="15.109375" customWidth="1"/>
-    <col min="27" max="27" width="14.21875" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" customWidth="1"/>
-    <col min="32" max="32" width="17.109375" customWidth="1"/>
-    <col min="33" max="33" width="12.6640625" customWidth="1"/>
-    <col min="37" max="37" width="17" customWidth="1"/>
-    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.88671875" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" customWidth="1"/>
+    <col min="27" max="27" width="12.7109375" customWidth="1"/>
+    <col min="29" max="29" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17" customWidth="1"/>
+    <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -3220,843 +3120,957 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD1" s="9" t="s">
+      <c r="V1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="Y1" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="Z1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>39</v>
+      </c>
       <c r="AF1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="AG1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AH1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AJ1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AK1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AL1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AM1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AN1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AO1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="AP1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="AQ1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AR1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="AS1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY1" t="s">
         <v>53</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="AT1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="AU1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="AV1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="AW1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="AX1" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>3.6542719566322601E-3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <v>-3.5907329753545297E-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="10">
         <v>4.0168535878294102E-2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>-7.8514873165093906E-3</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="10">
         <v>3.3935745189209998E-2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="10">
         <v>4.0576432751828498E-2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="10">
         <v>7.2072507506239197E-2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="10">
         <v>3.6049672164752203E-2</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="10">
         <v>6.4628140225999803E-2</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="10">
         <v>1.36432666452452E-2</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="10">
         <v>1.05856781581492E-2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="10">
         <v>2.85265547149419E-2</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="10">
         <v>5.0951836428762397E-3</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="10">
         <v>4.1643321660136103E-2</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="10">
         <v>5.23815692522707E-2</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="10">
         <v>2.7409751713423899E-2</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="10">
         <v>-3.61849905715729E-2</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="10">
         <v>-8.3272286863311604E-2</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="10">
         <v>2.2357020177426301E-2</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="10">
         <v>2.6569557742685899E-2</v>
       </c>
-      <c r="V2">
-        <v>6.1481108599952899E-2</v>
-      </c>
-      <c r="W2">
+      <c r="V2" s="10">
         <v>6.5646560875048401E-2</v>
       </c>
-      <c r="X2">
-        <v>6.8092356399512194E-2</v>
-      </c>
-      <c r="Y2">
-        <v>6.1132891107448503E-2</v>
-      </c>
-      <c r="Z2">
-        <v>6.1273540475592699E-2</v>
-      </c>
-      <c r="AA2">
+      <c r="W2" s="10">
         <v>7.0640785404322504E-2</v>
       </c>
-      <c r="AB2">
-        <v>6.98645385732755E-2</v>
-      </c>
-      <c r="AC2">
-        <v>6.5152951196098499E-2</v>
-      </c>
-      <c r="AD2">
+      <c r="X2" s="10">
         <v>8.58017470943492E-3</v>
       </c>
-      <c r="AE2">
+      <c r="Y2" s="10">
         <v>3.9880898627107003E-2</v>
       </c>
-      <c r="AF2">
+      <c r="Z2" s="10">
         <v>-5.0174216680903903E-2</v>
       </c>
-      <c r="AG2">
+      <c r="AA2" s="10">
         <v>-1.1115647914014801E-2</v>
       </c>
-      <c r="AH2">
+      <c r="AB2" s="10">
         <v>8.1620869725395201E-2</v>
       </c>
-      <c r="AI2">
+      <c r="AC2" s="10">
         <v>5.6542505230178598E-2</v>
       </c>
-      <c r="AJ2">
+      <c r="AD2" s="10">
         <v>2.0851764635020201E-2</v>
       </c>
-      <c r="AK2">
+      <c r="AE2" s="10">
         <v>-7.7958274690520496E-2</v>
       </c>
-      <c r="AL2">
+      <c r="AF2" s="10">
         <v>2.91139564172085E-2</v>
       </c>
-      <c r="AM2">
+      <c r="AG2" s="10">
         <v>4.4514296036975702E-2</v>
       </c>
-      <c r="AN2">
+      <c r="AH2" s="10">
         <v>4.62211879413673E-2</v>
       </c>
-      <c r="AO2">
+      <c r="AI2" s="10">
         <v>4.95125659931294E-2</v>
       </c>
-      <c r="AP2">
+      <c r="AJ2" s="10">
         <v>-3.9320203669231897E-2</v>
       </c>
-      <c r="AQ2">
+      <c r="AK2" s="10">
         <v>4.53550147261082E-2</v>
       </c>
-      <c r="AR2">
+      <c r="AL2" s="10">
         <v>6.8193671363391301E-2</v>
       </c>
-      <c r="AS2">
+      <c r="AM2" s="10">
         <v>5.9119838606919099E-2</v>
       </c>
-      <c r="AT2">
+      <c r="AN2" s="10">
         <v>5.6659822387717898E-2</v>
       </c>
-      <c r="AU2">
+      <c r="AO2" s="10">
         <v>-4.7899855357793099E-2</v>
       </c>
-      <c r="AV2">
+      <c r="AP2" s="10">
         <v>4.60747112231732E-2</v>
       </c>
-      <c r="AW2">
+      <c r="AQ2" s="10">
         <v>2.37270473547571E-2</v>
       </c>
-      <c r="AX2">
+      <c r="AR2" s="10">
         <v>7.54855050865616E-2</v>
       </c>
-      <c r="AY2">
+      <c r="AS2" s="10">
         <v>6.3655555568661995E-2</v>
       </c>
-      <c r="AZ2">
+      <c r="AT2" s="10">
         <v>-9.2370004325511897E-3</v>
       </c>
-      <c r="BA2">
+      <c r="AU2" s="10">
         <v>4.4839155309262503E-2</v>
       </c>
-      <c r="BB2">
+      <c r="AV2" s="10">
         <v>6.7932111226996798E-3</v>
       </c>
-      <c r="BC2">
+      <c r="AW2" s="10">
         <v>6.1611933564689601E-2</v>
       </c>
-      <c r="BD2">
+      <c r="AX2" s="10">
         <v>9.8244960503963502E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>4.5887719963423002E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>-4.61453738721792E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>9.1084154132544004E-2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <v>-3.6132267994944602E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <v>-0.13013650255276099</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="10">
         <v>8.8538040422745906E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="10">
         <v>0.18563891810785099</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="10">
         <v>0.18817828433514799</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="10">
         <v>0.13923824979596899</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="10">
         <v>7.7013935266935897E-3</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="10">
         <v>-6.2896327117740597E-2</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="10">
         <v>0.119842999797572</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="10">
         <v>8.3170594730998096E-2</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="10">
         <v>0.15534077985378</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="10">
         <v>0.15189723636577401</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="10">
         <v>0.142260153461888</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="10">
         <v>2.69951318376923E-2</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="10">
         <v>7.8596227469936802E-2</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="10">
         <v>8.4768682635347203E-2</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="10">
         <v>7.0501584816829305E-2</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="10">
         <v>7.1976264417725399E-3</v>
       </c>
-      <c r="W3">
-        <v>7.2921182600206899E-2</v>
-      </c>
-      <c r="X3">
-        <v>4.3448080174057699E-2</v>
-      </c>
-      <c r="Y3">
-        <v>4.8096646825785398E-2</v>
-      </c>
-      <c r="Z3" s="7">
+      <c r="W3" s="10">
         <v>-8.3930319562149696E-5</v>
       </c>
-      <c r="AA3">
-        <v>4.9274164565253999E-2</v>
-      </c>
-      <c r="AB3">
-        <v>3.7706264783932499E-2</v>
-      </c>
-      <c r="AC3">
-        <v>4.2886531516799498E-2</v>
-      </c>
-      <c r="AD3">
+      <c r="X3" s="10">
         <v>6.6789488196613303E-2</v>
       </c>
-      <c r="AE3">
+      <c r="Y3" s="10">
         <v>6.2360234115644599E-2</v>
       </c>
-      <c r="AF3">
+      <c r="Z3" s="10">
         <v>-0.13519685026174599</v>
       </c>
-      <c r="AG3">
+      <c r="AA3" s="10">
         <v>5.4070442205658299E-2</v>
       </c>
-      <c r="AH3">
+      <c r="AB3" s="10">
         <v>5.1081787852792902E-2</v>
       </c>
-      <c r="AI3">
+      <c r="AC3" s="10">
         <v>0.11894703546020299</v>
       </c>
-      <c r="AJ3">
+      <c r="AD3" s="10">
         <v>9.3365864393619699E-2</v>
       </c>
-      <c r="AK3">
+      <c r="AE3" s="10">
         <v>-8.4601981627773895E-2</v>
       </c>
-      <c r="AL3">
+      <c r="AF3" s="10">
         <v>4.0465368095723903E-2</v>
       </c>
-      <c r="AM3">
+      <c r="AG3" s="10">
         <v>6.7694506495493606E-2</v>
       </c>
-      <c r="AN3">
+      <c r="AH3" s="10">
         <v>0.101438235388758</v>
       </c>
-      <c r="AO3">
+      <c r="AI3" s="10">
         <v>0.126227153180589</v>
       </c>
-      <c r="AP3">
+      <c r="AJ3" s="10">
         <v>-7.9700561806794495E-2</v>
       </c>
-      <c r="AQ3">
+      <c r="AK3" s="10">
         <v>9.28284553314455E-2</v>
       </c>
-      <c r="AR3">
+      <c r="AL3" s="10">
         <v>9.6769807928780899E-2</v>
       </c>
-      <c r="AS3">
+      <c r="AM3" s="10">
         <v>7.5442868307704802E-2</v>
       </c>
-      <c r="AT3">
+      <c r="AN3" s="10">
         <v>9.9097597472187604E-2</v>
       </c>
-      <c r="AU3">
+      <c r="AO3" s="10">
         <v>-0.10847490584147899</v>
       </c>
-      <c r="AV3">
+      <c r="AP3" s="10">
         <v>0.116337147685878</v>
       </c>
-      <c r="AW3">
+      <c r="AQ3" s="10">
         <v>6.4110572809431096E-2</v>
       </c>
-      <c r="AX3">
+      <c r="AR3" s="10">
         <v>0.104089058174237</v>
       </c>
-      <c r="AY3">
+      <c r="AS3" s="10">
         <v>0.116110932896899</v>
       </c>
-      <c r="AZ3">
+      <c r="AT3" s="10">
         <v>7.5499954697417895E-2</v>
       </c>
-      <c r="BA3">
+      <c r="AU3" s="10">
         <v>0.130506509642517</v>
       </c>
-      <c r="BB3">
+      <c r="AV3" s="10">
         <v>8.6582029233284397E-2</v>
       </c>
-      <c r="BC3">
+      <c r="AW3" s="10">
         <v>4.2853176852960903E-2</v>
       </c>
-      <c r="BD3">
+      <c r="AX3" s="10">
         <v>8.6914290553508994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>2.9620942075363902E-3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>-3.1719545675779198E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="10">
         <v>7.8712677534828093E-2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="10">
         <v>9.7985682082775503E-3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="10">
         <v>-5.0508510473112E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="10">
         <v>6.2698947349680095E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="10">
         <v>0.115322259024822</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="10">
         <v>0.103549984786141</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="10">
         <v>9.8099382555565703E-2</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="10">
         <v>1.70776943920906E-2</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="10">
         <v>-1.8267442442448299E-2</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="10">
         <v>7.5874787668369803E-2</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="10">
         <v>3.0719843555763699E-2</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="10">
         <v>9.7608621073520793E-2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="10">
         <v>0.102208699892421</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="10">
         <v>7.4401630652462802E-2</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="10">
         <v>1.45394922526869E-2</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="10">
         <v>1.12212818055354E-2</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="10">
         <v>5.0872154194401997E-2</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="10">
         <v>5.2384768702153597E-2</v>
       </c>
-      <c r="V4">
-        <v>1.1155067232056899E-2</v>
-      </c>
-      <c r="W4">
-        <v>6.1736381334160199E-2</v>
-      </c>
-      <c r="X4">
+      <c r="V4" s="10">
         <v>4.2591077673404198E-2</v>
       </c>
-      <c r="Y4">
-        <v>3.06402233887243E-2</v>
-      </c>
-      <c r="Z4">
-        <v>1.9968149783343402E-2</v>
-      </c>
-      <c r="AA4">
-        <v>5.8511975453307698E-2</v>
-      </c>
-      <c r="AB4">
+      <c r="W4" s="10">
         <v>4.8646724504516001E-2</v>
       </c>
-      <c r="AC4">
-        <v>4.0916596902929099E-2</v>
-      </c>
-      <c r="AD4">
+      <c r="X4" s="10">
         <v>3.5644320438002003E-2</v>
       </c>
-      <c r="AE4">
+      <c r="Y4" s="10">
         <v>4.7768357152488498E-2</v>
       </c>
-      <c r="AF4">
+      <c r="Z4" s="10">
         <v>-7.4412943292753206E-2</v>
       </c>
-      <c r="AG4">
+      <c r="AA4" s="10">
         <v>1.4071551374656001E-2</v>
       </c>
-      <c r="AH4">
+      <c r="AB4" s="10">
         <v>8.7633691782178294E-2</v>
       </c>
-      <c r="AI4">
+      <c r="AC4" s="10">
         <v>7.02367851101727E-2</v>
       </c>
-      <c r="AJ4">
+      <c r="AD4" s="10">
         <v>6.1988022990964002E-2</v>
       </c>
-      <c r="AK4">
+      <c r="AE4" s="10">
         <v>-6.4842113190261605E-2</v>
       </c>
-      <c r="AL4">
+      <c r="AF4" s="10">
         <v>3.5473881450499602E-2</v>
       </c>
-      <c r="AM4">
+      <c r="AG4" s="10">
         <v>4.4174909880962003E-2</v>
       </c>
-      <c r="AN4">
+      <c r="AH4" s="10">
         <v>6.7230824384120896E-2</v>
       </c>
-      <c r="AO4">
+      <c r="AI4" s="10">
         <v>7.9550917204459795E-2</v>
       </c>
-      <c r="AP4">
+      <c r="AJ4" s="10">
         <v>-5.1243031048930202E-2</v>
       </c>
-      <c r="AQ4">
+      <c r="AK4" s="10">
         <v>7.4206711569888201E-2</v>
       </c>
-      <c r="AR4">
+      <c r="AL4" s="10">
         <v>7.9606240007111695E-2</v>
       </c>
-      <c r="AS4">
+      <c r="AM4" s="10">
         <v>6.6168884671081202E-2</v>
       </c>
-      <c r="AT4">
+      <c r="AN4" s="10">
         <v>8.2521538337383599E-2</v>
       </c>
-      <c r="AU4">
+      <c r="AO4" s="10">
         <v>-7.8355657968567902E-2</v>
       </c>
-      <c r="AV4">
+      <c r="AP4" s="10">
         <v>9.7050971734552599E-2</v>
       </c>
-      <c r="AW4">
+      <c r="AQ4" s="10">
         <v>6.3297726816497896E-2</v>
       </c>
-      <c r="AX4">
+      <c r="AR4" s="10">
         <v>9.4415429315916899E-2</v>
       </c>
-      <c r="AY4">
+      <c r="AS4" s="10">
         <v>9.7468579926351398E-2</v>
       </c>
-      <c r="AZ4">
+      <c r="AT4" s="10">
         <v>2.70090406031551E-2</v>
       </c>
-      <c r="BA4">
+      <c r="AU4" s="10">
         <v>6.2492124630612697E-2</v>
       </c>
-      <c r="BB4">
+      <c r="AV4" s="10">
         <v>3.6361318005219599E-2</v>
       </c>
-      <c r="BC4">
+      <c r="AW4" s="10">
         <v>7.65363237260068E-2</v>
       </c>
-      <c r="BD4">
+      <c r="AX4" s="10">
         <v>0.10552660541681499</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>1.7979414471414899E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>-2.3236976381542901E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="10">
         <v>6.9642397338041798E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10">
         <v>1.4443126740854901E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="10">
         <v>-6.8608494443085002E-3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="10">
         <v>6.1435442141734201E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="10">
         <v>0.107337587685576</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="10">
         <v>9.0542332785982504E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="10">
         <v>8.6220330993833694E-2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="10">
         <v>1.2926548018921799E-2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="10">
         <v>-8.0779614829628397E-3</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="10">
         <v>6.7715554980600903E-2</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="10">
         <v>2.9262461483508601E-2</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="10">
         <v>7.6173574026435598E-2</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="10">
         <v>9.7705330011313402E-2</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="10">
         <v>7.0942655512015604E-2</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="10">
         <v>1.11693978377718E-3</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="10">
         <v>-4.98908318445566E-3</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="10">
         <v>6.0564048654212999E-2</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="10">
         <v>4.5242070962676503E-2</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="10">
+        <v>6.0536205243669899E-2</v>
+      </c>
+      <c r="W5" s="10">
+        <v>6.4052650391340601E-2</v>
+      </c>
+      <c r="X5" s="10">
+        <v>2.67451658317415E-2</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>2.2219735308531101E-2</v>
+      </c>
+      <c r="Z5" s="10">
+        <v>-8.3733021909191796E-2</v>
+      </c>
+      <c r="AA5" s="10">
+        <v>1.2726439759369899E-2</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>8.3436651744581994E-2</v>
+      </c>
+      <c r="AC5" s="10">
+        <v>8.2790535331673604E-2</v>
+      </c>
+      <c r="AD5" s="10">
+        <v>4.8850389435154899E-2</v>
+      </c>
+      <c r="AE5" s="10">
+        <v>-5.5193079745180701E-2</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>2.40323447399312E-2</v>
+      </c>
+      <c r="AG5" s="10">
+        <v>6.0016952766866999E-2</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>6.7115006024987101E-2</v>
+      </c>
+      <c r="AI5" s="10">
+        <v>7.5039014542786595E-2</v>
+      </c>
+      <c r="AJ5" s="10">
+        <v>-5.6518487053646399E-2</v>
+      </c>
+      <c r="AK5" s="10">
+        <v>6.7960817767301604E-2</v>
+      </c>
+      <c r="AL5" s="10">
+        <v>8.2095249927299899E-2</v>
+      </c>
+      <c r="AM5" s="10">
+        <v>8.2739840400386802E-2</v>
+      </c>
+      <c r="AN5" s="10">
+        <v>9.2084831727734198E-2</v>
+      </c>
+      <c r="AO5" s="10">
+        <v>-6.0975498978436203E-2</v>
+      </c>
+      <c r="AP5" s="10">
+        <v>8.4555179605055597E-2</v>
+      </c>
+      <c r="AQ5" s="10">
+        <v>5.3069934222723901E-2</v>
+      </c>
+      <c r="AR5" s="10">
+        <v>9.6653226739949902E-2</v>
+      </c>
+      <c r="AS5" s="10">
+        <v>9.2544626077436895E-2</v>
+      </c>
+      <c r="AT5" s="10">
+        <v>2.39649842959853E-2</v>
+      </c>
+      <c r="AU5" s="10">
+        <v>6.8122027873895097E-2</v>
+      </c>
+      <c r="AV5" s="10">
+        <v>3.3862178508328698E-2</v>
+      </c>
+      <c r="AW5" s="10">
+        <v>6.0683414215142097E-2</v>
+      </c>
+      <c r="AX5" s="10">
+        <v>0.14602131985779701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="W15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="W16" s="10">
+        <v>6.1273540475592699E-2</v>
+      </c>
+      <c r="X16" s="10">
+        <v>7.0640785404322504E-2</v>
+      </c>
+      <c r="Y16" s="10">
+        <v>6.98645385732755E-2</v>
+      </c>
+      <c r="Z16" s="10">
+        <v>6.5152951196098499E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="W17" s="10">
+        <v>-8.3930319562149696E-5</v>
+      </c>
+      <c r="X17" s="10">
+        <v>4.9274164565253999E-2</v>
+      </c>
+      <c r="Y17" s="10">
+        <v>3.7706264783932499E-2</v>
+      </c>
+      <c r="Z17" s="10">
+        <v>4.2886531516799498E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="W18" s="10">
+        <v>1.9968149783343402E-2</v>
+      </c>
+      <c r="X18" s="10">
+        <v>5.8511975453307698E-2</v>
+      </c>
+      <c r="Y18" s="10">
+        <v>4.8646724504516001E-2</v>
+      </c>
+      <c r="Z18" s="10">
+        <v>4.0916596902929099E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="W19" s="10">
+        <v>3.4612962347062001E-2</v>
+      </c>
+      <c r="X19" s="10">
+        <v>6.0889863328223E-2</v>
+      </c>
+      <c r="Y19" s="10">
+        <v>5.7303160829740997E-2</v>
+      </c>
+      <c r="Z19" s="10">
+        <v>6.4052650391340601E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="W21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="X21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="W22" s="10">
+        <v>6.1481108599952899E-2</v>
+      </c>
+      <c r="X22" s="10">
+        <v>6.5646560875048401E-2</v>
+      </c>
+      <c r="Y22" s="10">
+        <v>6.8092356399512194E-2</v>
+      </c>
+      <c r="Z22" s="10">
+        <v>6.1132891107448503E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="W23" s="10">
+        <v>7.1976264417725399E-3</v>
+      </c>
+      <c r="X23" s="10">
+        <v>7.2921182600206899E-2</v>
+      </c>
+      <c r="Y23" s="10">
+        <v>4.3448080174057699E-2</v>
+      </c>
+      <c r="Z23" s="10">
+        <v>4.8096646825785398E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="W24" s="10">
+        <v>1.1155067232056899E-2</v>
+      </c>
+      <c r="X24" s="10">
+        <v>6.1736381334160199E-2</v>
+      </c>
+      <c r="Y24" s="10">
+        <v>4.2591077673404198E-2</v>
+      </c>
+      <c r="Z24" s="10">
+        <v>3.06402233887243E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="W25" s="10">
         <v>3.6551489208771298E-2</v>
       </c>
-      <c r="W5">
+      <c r="X25" s="10">
         <v>6.6462920640241299E-2</v>
       </c>
-      <c r="X5">
+      <c r="Y25" s="10">
         <v>5.66946672272527E-2</v>
       </c>
-      <c r="Y5">
+      <c r="Z25" s="10">
         <v>6.0536205243669899E-2</v>
       </c>
-      <c r="Z5">
-        <v>3.4612962347062001E-2</v>
-      </c>
-      <c r="AA5">
-        <v>6.0889863328223E-2</v>
-      </c>
-      <c r="AB5">
-        <v>5.7303160829740997E-2</v>
-      </c>
-      <c r="AC5">
-        <v>6.4052650391340601E-2</v>
-      </c>
-      <c r="AD5">
-        <v>2.67451658317415E-2</v>
-      </c>
-      <c r="AE5">
-        <v>2.2219735308531101E-2</v>
-      </c>
-      <c r="AF5">
-        <v>-8.3733021909191796E-2</v>
-      </c>
-      <c r="AG5">
-        <v>1.2726439759369899E-2</v>
-      </c>
-      <c r="AH5">
-        <v>8.3436651744581994E-2</v>
-      </c>
-      <c r="AI5">
-        <v>8.2790535331673604E-2</v>
-      </c>
-      <c r="AJ5">
-        <v>4.8850389435154899E-2</v>
-      </c>
-      <c r="AK5">
-        <v>-5.5193079745180701E-2</v>
-      </c>
-      <c r="AL5">
-        <v>2.40323447399312E-2</v>
-      </c>
-      <c r="AM5">
-        <v>6.0016952766866999E-2</v>
-      </c>
-      <c r="AN5">
-        <v>6.7115006024987101E-2</v>
-      </c>
-      <c r="AO5">
-        <v>7.5039014542786595E-2</v>
-      </c>
-      <c r="AP5">
-        <v>-5.6518487053646399E-2</v>
-      </c>
-      <c r="AQ5">
-        <v>6.7960817767301604E-2</v>
-      </c>
-      <c r="AR5">
-        <v>8.2095249927299899E-2</v>
-      </c>
-      <c r="AS5">
-        <v>8.2739840400386802E-2</v>
-      </c>
-      <c r="AT5">
-        <v>9.2084831727734198E-2</v>
-      </c>
-      <c r="AU5">
-        <v>-6.0975498978436203E-2</v>
-      </c>
-      <c r="AV5">
-        <v>8.4555179605055597E-2</v>
-      </c>
-      <c r="AW5">
-        <v>5.3069934222723901E-2</v>
-      </c>
-      <c r="AX5">
-        <v>9.6653226739949902E-2</v>
-      </c>
-      <c r="AY5">
-        <v>9.2544626077436895E-2</v>
-      </c>
-      <c r="AZ5">
-        <v>2.39649842959853E-2</v>
-      </c>
-      <c r="BA5">
-        <v>6.8122027873895097E-2</v>
-      </c>
-      <c r="BB5">
-        <v>3.3862178508328698E-2</v>
-      </c>
-      <c r="BC5">
-        <v>6.0683414215142097E-2</v>
-      </c>
-      <c r="BD5">
-        <v>0.14602131985779701</v>
-      </c>
+    </row>
+    <row r="26" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:BD5">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="W21:Z25 W15:Z19 A1:AX5">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4075,23 +4089,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="5.77734375" style="1"/>
-    <col min="6" max="6" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="5.77734375" style="1"/>
-    <col min="15" max="15" width="5.77734375" style="4"/>
-    <col min="16" max="17" width="5.77734375" style="3"/>
-    <col min="18" max="18" width="5.77734375" style="6"/>
-    <col min="19" max="19" width="5.77734375" style="3"/>
-    <col min="20" max="16384" width="5.77734375" style="1"/>
+    <col min="1" max="3" width="5.7109375" style="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1"/>
+    <col min="6" max="6" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="5.7109375" style="1"/>
+    <col min="15" max="15" width="5.7109375" style="4"/>
+    <col min="16" max="17" width="5.7109375" style="3"/>
+    <col min="18" max="18" width="5.7109375" style="6"/>
+    <col min="19" max="19" width="5.7109375" style="3"/>
+    <col min="20" max="16384" width="5.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -4100,7 +4116,7 @@
       <c r="R1" s="5"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4279,7 +4295,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -4461,7 +4477,7 @@
         <v>8.46741608753801E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -4643,7 +4659,7 @@
         <v>0.222805115317015</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -4825,7 +4841,7 @@
         <v>0.27014514416885799</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -5007,12 +5023,12 @@
         <v>4.4311601195437204E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -5191,7 +5207,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -5373,7 +5389,7 @@
         <v>5.6490643111989598E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -5555,7 +5571,7 @@
         <v>5.8912854976812201E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -5737,7 +5753,7 @@
         <v>0.110091525151573</v>
       </c>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -5919,12 +5935,12 @@
         <v>4.3814894711411902E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
@@ -6103,7 +6119,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
@@ -6285,7 +6301,7 @@
         <v>7.3019696289745806E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
@@ -6467,7 +6483,7 @@
         <v>0.107859107012096</v>
       </c>
     </row>
-    <row r="24" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -6649,7 +6665,7 @@
         <v>7.5801871320471698E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -6856,14 +6872,14 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -7042,7 +7058,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -7224,7 +7240,7 @@
         <v>8.46741608753801E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -7406,7 +7422,7 @@
         <v>4.4311601195437204E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -7588,7 +7604,7 @@
         <v>0.222805115317015</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -7770,12 +7786,12 @@
         <v>0.27014514416885799</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -7954,7 +7970,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -8136,7 +8152,7 @@
         <v>5.6490643111989598E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -8318,7 +8334,7 @@
         <v>1.8376308666780399E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -8500,7 +8516,7 @@
         <v>5.6728986744919899E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -8682,12 +8698,12 @@
         <v>0.110393068985955</v>
       </c>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -8866,7 +8882,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -9048,7 +9064,7 @@
         <v>7.3019696289745806E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -9230,7 +9246,7 @@
         <v>7.9234979480474907E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -9412,7 +9428,7 @@
         <v>0.107859107012096</v>
       </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -9653,14 +9669,14 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -9851,7 +9867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -10045,7 +10061,7 @@
         <v>3.29370682531262E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -10239,7 +10255,7 @@
         <v>0.38217754224887401</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -10433,7 +10449,7 @@
         <v>0.24374232010933999</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -10627,12 +10643,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -10823,7 +10839,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -11017,7 +11033,7 @@
         <v>0.46885123253798999</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -11211,7 +11227,7 @@
         <v>0.34933916655896202</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -11405,7 +11421,7 @@
         <v>0.453037315572413</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -11599,12 +11615,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -11795,7 +11811,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -11989,7 +12005,7 @@
         <v>0.21791509577485399</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -12183,7 +12199,7 @@
         <v>0.36488943428878101</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -12377,7 +12393,7 @@
         <v>0.34906855275703702</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -12584,14 +12600,14 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -12782,7 +12798,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -12976,7 +12992,7 @@
         <v>3.29370682531262E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -13170,7 +13186,7 @@
         <v>0.38217754224887401</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -13364,7 +13380,7 @@
         <v>0.24374232010933999</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -13558,12 +13574,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -13754,7 +13770,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -13948,7 +13964,7 @@
         <v>0.46885123253798999</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -14142,7 +14158,7 @@
         <v>0.34933916655896202</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -14336,7 +14352,7 @@
         <v>0.453037315572413</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -14530,12 +14546,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -14726,7 +14742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -14920,7 +14936,7 @@
         <v>0.21791509577485399</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -15114,7 +15130,7 @@
         <v>0.36488943428878101</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -15308,7 +15324,7 @@
         <v>0.34906855275703702</v>
       </c>
     </row>
-    <row r="25" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -15515,14 +15531,14 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -15713,7 +15729,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -15907,7 +15923,7 @@
         <v>3.29370682531262E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -16101,7 +16117,7 @@
         <v>0.38217754224887401</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -16295,7 +16311,7 @@
         <v>0.24374232010933999</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -16489,12 +16505,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -16685,7 +16701,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -16879,7 +16895,7 @@
         <v>0.46885123253798999</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -17073,7 +17089,7 @@
         <v>0.34933916655896202</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -17267,7 +17283,7 @@
         <v>0.453037315572413</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -17461,12 +17477,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -17657,7 +17673,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -17851,7 +17867,7 @@
         <v>0.21791509577485399</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -18045,7 +18061,7 @@
         <v>0.36488943428878101</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -18239,7 +18255,7 @@
         <v>0.34906855275703702</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>

</xml_diff>